<commit_message>
added rule-based agent capability and testing loop
</commit_message>
<xml_diff>
--- a/run-data.xlsx
+++ b/run-data.xlsx
@@ -14,20 +14,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
-  <si>
-    <t>rollout</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>rew</t>
   </si>
   <si>
     <t>waitingTime</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>rew</t>
-  </si>
-  <si>
     <t>E_num_train_rollouts</t>
   </si>
   <si>
@@ -91,7 +88,10 @@
     <t>O_rule_set_params</t>
   </si>
   <si>
-    <t>{'length': 30}</t>
+    <t>timer</t>
+  </si>
+  <si>
+    <t>{'length': 10}</t>
   </si>
 </sst>
 </file>
@@ -449,13 +449,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,155 +528,78 @@
       <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:24">
       <c r="A2">
+        <v>0.1966046134630839</v>
+      </c>
+      <c r="B2">
+        <v>870.8666666666667</v>
+      </c>
+      <c r="C2">
+        <v>12.69385964912281</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>64</v>
+      </c>
+      <c r="F2">
         <v>5</v>
-      </c>
-      <c r="B2">
-        <v>28.5</v>
-      </c>
-      <c r="C2">
-        <v>0.2001784046490987</v>
-      </c>
-      <c r="D2">
-        <v>762</v>
-      </c>
-      <c r="E2">
-        <v>20</v>
-      </c>
-      <c r="F2">
-        <v>64</v>
       </c>
       <c r="G2">
         <v>5</v>
       </c>
       <c r="H2">
+        <v>250</v>
+      </c>
+      <c r="I2">
+        <v>20</v>
+      </c>
+      <c r="J2">
+        <v>6</v>
+      </c>
+      <c r="K2">
         <v>2</v>
       </c>
-      <c r="I2">
-        <v>250</v>
-      </c>
-      <c r="J2">
-        <v>50</v>
-      </c>
-      <c r="K2">
-        <v>6</v>
-      </c>
       <c r="L2">
-        <v>2</v>
+        <v>0.9</v>
       </c>
       <c r="M2">
-        <v>0.9</v>
+        <v>0.01</v>
       </c>
       <c r="N2">
-        <v>0.01</v>
+        <v>32</v>
       </c>
       <c r="O2">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="P2">
-        <v>10</v>
+        <v>0.3</v>
       </c>
       <c r="Q2">
-        <v>0.3</v>
+        <v>0.99</v>
       </c>
       <c r="R2">
-        <v>0.99</v>
-      </c>
-      <c r="S2">
         <v>0.001</v>
       </c>
-      <c r="T2" t="b">
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2">
         <v>1</v>
       </c>
       <c r="U2">
         <v>1</v>
       </c>
       <c r="V2">
-        <v>1</v>
-      </c>
-      <c r="W2">
-        <v>1</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25">
-      <c r="A3">
-        <v>20</v>
-      </c>
-      <c r="B3">
-        <v>8.375</v>
-      </c>
-      <c r="C3">
-        <v>0.2023764848709106</v>
-      </c>
-      <c r="D3">
-        <v>900</v>
-      </c>
-      <c r="E3">
-        <v>20</v>
-      </c>
-      <c r="F3">
-        <v>64</v>
-      </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>250</v>
-      </c>
-      <c r="J3">
-        <v>50</v>
-      </c>
-      <c r="K3">
-        <v>6</v>
-      </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
-      <c r="M3">
-        <v>0.9</v>
-      </c>
-      <c r="N3">
-        <v>0.01</v>
-      </c>
-      <c r="O3">
-        <v>32</v>
-      </c>
-      <c r="P3">
-        <v>10</v>
-      </c>
-      <c r="Q3">
-        <v>0.3</v>
-      </c>
-      <c r="R3">
-        <v>0.99</v>
-      </c>
-      <c r="S3">
-        <v>0.001</v>
-      </c>
-      <c r="T3" t="b">
-        <v>1</v>
-      </c>
-      <c r="U3">
-        <v>1</v>
-      </c>
-      <c r="V3">
-        <v>1</v>
-      </c>
-      <c r="W3">
-        <v>1</v>
-      </c>
-      <c r="Y3" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2" t="s">
+        <v>24</v>
+      </c>
+      <c r="X2" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added random and grid hyperparam searching
</commit_message>
<xml_diff>
--- a/run-data.xlsx
+++ b/run-data.xlsx
@@ -531,13 +531,13 @@
     </row>
     <row r="2" spans="1:24">
       <c r="A2">
-        <v>0.1966046134630839</v>
+        <v>0.1816669225692749</v>
       </c>
       <c r="B2">
-        <v>870.8666666666667</v>
+        <v>542.2857142857143</v>
       </c>
       <c r="C2">
-        <v>12.69385964912281</v>
+        <v>5.978195488721804</v>
       </c>
       <c r="D2">
         <v>20</v>
@@ -552,10 +552,10 @@
         <v>5</v>
       </c>
       <c r="H2">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="I2">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J2">
         <v>6</v>
@@ -567,7 +567,7 @@
         <v>0.9</v>
       </c>
       <c r="M2">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="N2">
         <v>32</v>
@@ -594,7 +594,7 @@
         <v>1</v>
       </c>
       <c r="V2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="W2" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
added saving/loading for model weights for testing
</commit_message>
<xml_diff>
--- a/run-data.xlsx
+++ b/run-data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>time</t>
   </si>
@@ -86,12 +86,6 @@
   </si>
   <si>
     <t>O_rule_set_params</t>
-  </si>
-  <si>
-    <t>timer</t>
-  </si>
-  <si>
-    <t>{'length': 10}</t>
   </si>
 </sst>
 </file>
@@ -449,7 +443,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -529,80 +523,6 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
-      <c r="A2">
-        <v>0.1816669225692749</v>
-      </c>
-      <c r="B2">
-        <v>542.2857142857143</v>
-      </c>
-      <c r="C2">
-        <v>5.978195488721804</v>
-      </c>
-      <c r="D2">
-        <v>20</v>
-      </c>
-      <c r="E2">
-        <v>64</v>
-      </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <v>150</v>
-      </c>
-      <c r="I2">
-        <v>15</v>
-      </c>
-      <c r="J2">
-        <v>6</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-      <c r="L2">
-        <v>0.9</v>
-      </c>
-      <c r="M2">
-        <v>0.05</v>
-      </c>
-      <c r="N2">
-        <v>32</v>
-      </c>
-      <c r="O2">
-        <v>10</v>
-      </c>
-      <c r="P2">
-        <v>0.3</v>
-      </c>
-      <c r="Q2">
-        <v>0.99</v>
-      </c>
-      <c r="R2">
-        <v>0.001</v>
-      </c>
-      <c r="S2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <v>1</v>
-      </c>
-      <c r="V2">
-        <v>5</v>
-      </c>
-      <c r="W2" t="s">
-        <v>24</v>
-      </c>
-      <c r="X2" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added four intersection env and multi intersection rule-based model
</commit_message>
<xml_diff>
--- a/run-data.xlsx
+++ b/run-data.xlsx
@@ -14,20 +14,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>rollout</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>rew</t>
   </si>
   <si>
     <t>waitingTime</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>rew</t>
-  </si>
-  <si>
     <t>E_num_train_rollouts</t>
   </si>
   <si>
@@ -43,15 +40,12 @@
     <t>E_max_ep_steps</t>
   </si>
   <si>
+    <t>E_generation_ep_steps</t>
+  </si>
+  <si>
     <t>E_test_num_eps</t>
   </si>
   <si>
-    <t>M_state_size</t>
-  </si>
-  <si>
-    <t>M_action_size</t>
-  </si>
-  <si>
     <t>A_gae_tau</t>
   </si>
   <si>
@@ -89,6 +83,18 @@
   </si>
   <si>
     <t>O_rule_set_params</t>
+  </si>
+  <si>
+    <t>O_environment</t>
+  </si>
+  <si>
+    <t>O_NS_mult</t>
+  </si>
+  <si>
+    <t>O_EW_mult</t>
+  </si>
+  <si>
+    <t>O_phase_end_offset</t>
   </si>
 </sst>
 </file>
@@ -446,13 +452,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:27">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,6 +533,12 @@
       </c>
       <c r="Y1" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tuned agent on multi-intersection
</commit_message>
<xml_diff>
--- a/run-data.xlsx
+++ b/run-data.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+  <si>
+    <t>rollout</t>
+  </si>
+  <si>
+    <t>waitingTime</t>
+  </si>
   <si>
     <t>time</t>
   </si>
@@ -22,9 +28,6 @@
     <t>rew</t>
   </si>
   <si>
-    <t>waitingTime</t>
-  </si>
-  <si>
     <t>E_num_train_rollouts</t>
   </si>
   <si>
@@ -95,6 +98,12 @@
   </si>
   <si>
     <t>O_phase_end_offset</t>
+  </si>
+  <si>
+    <t>{'cycle_length': 20}</t>
+  </si>
+  <si>
+    <t>four_intersections</t>
   </si>
 </sst>
 </file>
@@ -452,13 +461,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AB17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,6 +548,1337 @@
       </c>
       <c r="AA1" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28">
+      <c r="A2">
+        <v>208</v>
+      </c>
+      <c r="B2">
+        <v>1861.870833333333</v>
+      </c>
+      <c r="C2">
+        <v>9.890320293108623</v>
+      </c>
+      <c r="D2">
+        <v>413.0110416666665</v>
+      </c>
+      <c r="E2">
+        <v>200</v>
+      </c>
+      <c r="F2">
+        <v>1024</v>
+      </c>
+      <c r="G2">
+        <v>48</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2">
+        <v>900</v>
+      </c>
+      <c r="J2">
+        <v>750</v>
+      </c>
+      <c r="K2">
+        <v>100</v>
+      </c>
+      <c r="L2">
+        <v>0.85</v>
+      </c>
+      <c r="M2">
+        <v>0.2</v>
+      </c>
+      <c r="N2">
+        <v>256</v>
+      </c>
+      <c r="O2">
+        <v>5</v>
+      </c>
+      <c r="P2">
+        <v>0.3</v>
+      </c>
+      <c r="Q2">
+        <v>0.99</v>
+      </c>
+      <c r="R2">
+        <v>0.0001</v>
+      </c>
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>8</v>
+      </c>
+      <c r="X2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z2">
+        <v>1.5</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28">
+      <c r="A3">
+        <v>208</v>
+      </c>
+      <c r="B3">
+        <v>1861.508333333333</v>
+      </c>
+      <c r="C3">
+        <v>10.05728667974472</v>
+      </c>
+      <c r="D3">
+        <v>414.7449999999998</v>
+      </c>
+      <c r="E3">
+        <v>200</v>
+      </c>
+      <c r="F3">
+        <v>1024</v>
+      </c>
+      <c r="G3">
+        <v>48</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
+      <c r="I3">
+        <v>900</v>
+      </c>
+      <c r="J3">
+        <v>750</v>
+      </c>
+      <c r="K3">
+        <v>100</v>
+      </c>
+      <c r="L3">
+        <v>0.85</v>
+      </c>
+      <c r="M3">
+        <v>0.2</v>
+      </c>
+      <c r="N3">
+        <v>256</v>
+      </c>
+      <c r="O3">
+        <v>5</v>
+      </c>
+      <c r="P3">
+        <v>0.3</v>
+      </c>
+      <c r="Q3">
+        <v>0.99</v>
+      </c>
+      <c r="R3">
+        <v>0.0001</v>
+      </c>
+      <c r="S3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>8</v>
+      </c>
+      <c r="X3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z3">
+        <v>1.5</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28">
+      <c r="A4">
+        <v>408</v>
+      </c>
+      <c r="B4">
+        <v>1840.322222222222</v>
+      </c>
+      <c r="C4">
+        <v>16.34709590276082</v>
+      </c>
+      <c r="D4">
+        <v>403.6943750000002</v>
+      </c>
+      <c r="E4">
+        <v>400</v>
+      </c>
+      <c r="F4">
+        <v>1024</v>
+      </c>
+      <c r="G4">
+        <v>48</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="I4">
+        <v>900</v>
+      </c>
+      <c r="J4">
+        <v>750</v>
+      </c>
+      <c r="K4">
+        <v>100</v>
+      </c>
+      <c r="L4">
+        <v>0.85</v>
+      </c>
+      <c r="M4">
+        <v>0.2</v>
+      </c>
+      <c r="N4">
+        <v>256</v>
+      </c>
+      <c r="O4">
+        <v>5</v>
+      </c>
+      <c r="P4">
+        <v>0.3</v>
+      </c>
+      <c r="Q4">
+        <v>0.99</v>
+      </c>
+      <c r="R4">
+        <v>0.0001</v>
+      </c>
+      <c r="S4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>8</v>
+      </c>
+      <c r="X4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z4">
+        <v>1.5</v>
+      </c>
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28">
+      <c r="A5">
+        <v>408</v>
+      </c>
+      <c r="B5">
+        <v>1843.663888888889</v>
+      </c>
+      <c r="C5">
+        <v>16.36791323026021</v>
+      </c>
+      <c r="D5">
+        <v>407.8318750000003</v>
+      </c>
+      <c r="E5">
+        <v>400</v>
+      </c>
+      <c r="F5">
+        <v>1024</v>
+      </c>
+      <c r="G5">
+        <v>48</v>
+      </c>
+      <c r="H5">
+        <v>30</v>
+      </c>
+      <c r="I5">
+        <v>900</v>
+      </c>
+      <c r="J5">
+        <v>750</v>
+      </c>
+      <c r="K5">
+        <v>100</v>
+      </c>
+      <c r="L5">
+        <v>0.85</v>
+      </c>
+      <c r="M5">
+        <v>0.2</v>
+      </c>
+      <c r="N5">
+        <v>256</v>
+      </c>
+      <c r="O5">
+        <v>5</v>
+      </c>
+      <c r="P5">
+        <v>0.3</v>
+      </c>
+      <c r="Q5">
+        <v>0.99</v>
+      </c>
+      <c r="R5">
+        <v>0.0001</v>
+      </c>
+      <c r="S5" t="b">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>8</v>
+      </c>
+      <c r="X5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z5">
+        <v>1.5</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28">
+      <c r="A6">
+        <v>144</v>
+      </c>
+      <c r="B6">
+        <v>1859.706944444444</v>
+      </c>
+      <c r="C6">
+        <v>17.37346264918645</v>
+      </c>
+      <c r="D6">
+        <v>416.6354166666667</v>
+      </c>
+      <c r="E6">
+        <v>200</v>
+      </c>
+      <c r="F6">
+        <v>2048</v>
+      </c>
+      <c r="G6">
+        <v>48</v>
+      </c>
+      <c r="H6">
+        <v>30</v>
+      </c>
+      <c r="I6">
+        <v>900</v>
+      </c>
+      <c r="J6">
+        <v>750</v>
+      </c>
+      <c r="K6">
+        <v>100</v>
+      </c>
+      <c r="L6">
+        <v>0.85</v>
+      </c>
+      <c r="M6">
+        <v>0.2</v>
+      </c>
+      <c r="N6">
+        <v>256</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
+      <c r="P6">
+        <v>0.3</v>
+      </c>
+      <c r="Q6">
+        <v>0.99</v>
+      </c>
+      <c r="R6">
+        <v>0.0001</v>
+      </c>
+      <c r="S6" t="b">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>8</v>
+      </c>
+      <c r="X6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z6">
+        <v>1.5</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28">
+      <c r="A7">
+        <v>208</v>
+      </c>
+      <c r="B7">
+        <v>1867.433333333333</v>
+      </c>
+      <c r="C7">
+        <v>17.24168705940247</v>
+      </c>
+      <c r="D7">
+        <v>421.0416666666667</v>
+      </c>
+      <c r="E7">
+        <v>200</v>
+      </c>
+      <c r="F7">
+        <v>2048</v>
+      </c>
+      <c r="G7">
+        <v>48</v>
+      </c>
+      <c r="H7">
+        <v>30</v>
+      </c>
+      <c r="I7">
+        <v>900</v>
+      </c>
+      <c r="J7">
+        <v>750</v>
+      </c>
+      <c r="K7">
+        <v>100</v>
+      </c>
+      <c r="L7">
+        <v>0.85</v>
+      </c>
+      <c r="M7">
+        <v>0.2</v>
+      </c>
+      <c r="N7">
+        <v>256</v>
+      </c>
+      <c r="O7">
+        <v>5</v>
+      </c>
+      <c r="P7">
+        <v>0.3</v>
+      </c>
+      <c r="Q7">
+        <v>0.99</v>
+      </c>
+      <c r="R7">
+        <v>0.0001</v>
+      </c>
+      <c r="S7" t="b">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <v>8</v>
+      </c>
+      <c r="X7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z7">
+        <v>1.5</v>
+      </c>
+      <c r="AA7">
+        <v>1</v>
+      </c>
+      <c r="AB7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28">
+      <c r="A8">
+        <v>408</v>
+      </c>
+      <c r="B8">
+        <v>1828.779166666667</v>
+      </c>
+      <c r="C8">
+        <v>29.75985050996145</v>
+      </c>
+      <c r="D8">
+        <v>416.3758333333334</v>
+      </c>
+      <c r="E8">
+        <v>400</v>
+      </c>
+      <c r="F8">
+        <v>2048</v>
+      </c>
+      <c r="G8">
+        <v>48</v>
+      </c>
+      <c r="H8">
+        <v>30</v>
+      </c>
+      <c r="I8">
+        <v>900</v>
+      </c>
+      <c r="J8">
+        <v>750</v>
+      </c>
+      <c r="K8">
+        <v>100</v>
+      </c>
+      <c r="L8">
+        <v>0.85</v>
+      </c>
+      <c r="M8">
+        <v>0.2</v>
+      </c>
+      <c r="N8">
+        <v>256</v>
+      </c>
+      <c r="O8">
+        <v>5</v>
+      </c>
+      <c r="P8">
+        <v>0.3</v>
+      </c>
+      <c r="Q8">
+        <v>0.99</v>
+      </c>
+      <c r="R8">
+        <v>0.0001</v>
+      </c>
+      <c r="S8" t="b">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>8</v>
+      </c>
+      <c r="X8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z8">
+        <v>1.5</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28">
+      <c r="A9">
+        <v>336</v>
+      </c>
+      <c r="B9">
+        <v>1812.058333333333</v>
+      </c>
+      <c r="C9">
+        <v>29.9301810781161</v>
+      </c>
+      <c r="D9">
+        <v>418.3845833333334</v>
+      </c>
+      <c r="E9">
+        <v>400</v>
+      </c>
+      <c r="F9">
+        <v>2048</v>
+      </c>
+      <c r="G9">
+        <v>48</v>
+      </c>
+      <c r="H9">
+        <v>30</v>
+      </c>
+      <c r="I9">
+        <v>900</v>
+      </c>
+      <c r="J9">
+        <v>750</v>
+      </c>
+      <c r="K9">
+        <v>100</v>
+      </c>
+      <c r="L9">
+        <v>0.85</v>
+      </c>
+      <c r="M9">
+        <v>0.2</v>
+      </c>
+      <c r="N9">
+        <v>256</v>
+      </c>
+      <c r="O9">
+        <v>5</v>
+      </c>
+      <c r="P9">
+        <v>0.3</v>
+      </c>
+      <c r="Q9">
+        <v>0.99</v>
+      </c>
+      <c r="R9">
+        <v>0.0001</v>
+      </c>
+      <c r="S9" t="b">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9">
+        <v>8</v>
+      </c>
+      <c r="X9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z9">
+        <v>1.5</v>
+      </c>
+      <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AB9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28">
+      <c r="A10">
+        <v>208</v>
+      </c>
+      <c r="B10">
+        <v>2236.4375</v>
+      </c>
+      <c r="C10">
+        <v>10.08121913671494</v>
+      </c>
+      <c r="D10">
+        <v>425.2495833333334</v>
+      </c>
+      <c r="E10">
+        <v>200</v>
+      </c>
+      <c r="F10">
+        <v>1024</v>
+      </c>
+      <c r="G10">
+        <v>48</v>
+      </c>
+      <c r="H10">
+        <v>30</v>
+      </c>
+      <c r="I10">
+        <v>900</v>
+      </c>
+      <c r="J10">
+        <v>750</v>
+      </c>
+      <c r="K10">
+        <v>100</v>
+      </c>
+      <c r="L10">
+        <v>0.85</v>
+      </c>
+      <c r="M10">
+        <v>0.2</v>
+      </c>
+      <c r="N10">
+        <v>256</v>
+      </c>
+      <c r="O10">
+        <v>5</v>
+      </c>
+      <c r="P10">
+        <v>0.3</v>
+      </c>
+      <c r="Q10">
+        <v>0.99</v>
+      </c>
+      <c r="R10">
+        <v>1e-05</v>
+      </c>
+      <c r="S10" t="b">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>8</v>
+      </c>
+      <c r="X10" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z10">
+        <v>1.5</v>
+      </c>
+      <c r="AA10">
+        <v>1</v>
+      </c>
+      <c r="AB10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28">
+      <c r="A11">
+        <v>208</v>
+      </c>
+      <c r="B11">
+        <v>3399.819444444444</v>
+      </c>
+      <c r="C11">
+        <v>10.13506108522415</v>
+      </c>
+      <c r="D11">
+        <v>369.8535416666668</v>
+      </c>
+      <c r="E11">
+        <v>200</v>
+      </c>
+      <c r="F11">
+        <v>1024</v>
+      </c>
+      <c r="G11">
+        <v>48</v>
+      </c>
+      <c r="H11">
+        <v>30</v>
+      </c>
+      <c r="I11">
+        <v>900</v>
+      </c>
+      <c r="J11">
+        <v>750</v>
+      </c>
+      <c r="K11">
+        <v>100</v>
+      </c>
+      <c r="L11">
+        <v>0.85</v>
+      </c>
+      <c r="M11">
+        <v>0.2</v>
+      </c>
+      <c r="N11">
+        <v>256</v>
+      </c>
+      <c r="O11">
+        <v>5</v>
+      </c>
+      <c r="P11">
+        <v>0.3</v>
+      </c>
+      <c r="Q11">
+        <v>0.99</v>
+      </c>
+      <c r="R11">
+        <v>1e-05</v>
+      </c>
+      <c r="S11" t="b">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <v>8</v>
+      </c>
+      <c r="X11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z11">
+        <v>1.5</v>
+      </c>
+      <c r="AA11">
+        <v>1</v>
+      </c>
+      <c r="AB11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28">
+      <c r="A12">
+        <v>408</v>
+      </c>
+      <c r="B12">
+        <v>1937.751388888889</v>
+      </c>
+      <c r="C12">
+        <v>16.26151429414749</v>
+      </c>
+      <c r="D12">
+        <v>404.0227083333332</v>
+      </c>
+      <c r="E12">
+        <v>400</v>
+      </c>
+      <c r="F12">
+        <v>1024</v>
+      </c>
+      <c r="G12">
+        <v>48</v>
+      </c>
+      <c r="H12">
+        <v>30</v>
+      </c>
+      <c r="I12">
+        <v>900</v>
+      </c>
+      <c r="J12">
+        <v>750</v>
+      </c>
+      <c r="K12">
+        <v>100</v>
+      </c>
+      <c r="L12">
+        <v>0.85</v>
+      </c>
+      <c r="M12">
+        <v>0.2</v>
+      </c>
+      <c r="N12">
+        <v>256</v>
+      </c>
+      <c r="O12">
+        <v>5</v>
+      </c>
+      <c r="P12">
+        <v>0.3</v>
+      </c>
+      <c r="Q12">
+        <v>0.99</v>
+      </c>
+      <c r="R12">
+        <v>1e-05</v>
+      </c>
+      <c r="S12" t="b">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <v>8</v>
+      </c>
+      <c r="X12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z12">
+        <v>1.5</v>
+      </c>
+      <c r="AA12">
+        <v>1</v>
+      </c>
+      <c r="AB12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28">
+      <c r="A13">
+        <v>408</v>
+      </c>
+      <c r="B13">
+        <v>2042.166666666667</v>
+      </c>
+      <c r="C13">
+        <v>16.51061455011368</v>
+      </c>
+      <c r="D13">
+        <v>421.1222916666667</v>
+      </c>
+      <c r="E13">
+        <v>400</v>
+      </c>
+      <c r="F13">
+        <v>1024</v>
+      </c>
+      <c r="G13">
+        <v>48</v>
+      </c>
+      <c r="H13">
+        <v>30</v>
+      </c>
+      <c r="I13">
+        <v>900</v>
+      </c>
+      <c r="J13">
+        <v>750</v>
+      </c>
+      <c r="K13">
+        <v>100</v>
+      </c>
+      <c r="L13">
+        <v>0.85</v>
+      </c>
+      <c r="M13">
+        <v>0.2</v>
+      </c>
+      <c r="N13">
+        <v>256</v>
+      </c>
+      <c r="O13">
+        <v>5</v>
+      </c>
+      <c r="P13">
+        <v>0.3</v>
+      </c>
+      <c r="Q13">
+        <v>0.99</v>
+      </c>
+      <c r="R13">
+        <v>1e-05</v>
+      </c>
+      <c r="S13" t="b">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
+      <c r="V13">
+        <v>8</v>
+      </c>
+      <c r="X13" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z13">
+        <v>1.5</v>
+      </c>
+      <c r="AA13">
+        <v>1</v>
+      </c>
+      <c r="AB13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28">
+      <c r="A14">
+        <v>48</v>
+      </c>
+      <c r="B14">
+        <v>1899.809722222222</v>
+      </c>
+      <c r="C14">
+        <v>17.10914916197459</v>
+      </c>
+      <c r="D14">
+        <v>420.0268750000001</v>
+      </c>
+      <c r="E14">
+        <v>200</v>
+      </c>
+      <c r="F14">
+        <v>2048</v>
+      </c>
+      <c r="G14">
+        <v>48</v>
+      </c>
+      <c r="H14">
+        <v>30</v>
+      </c>
+      <c r="I14">
+        <v>900</v>
+      </c>
+      <c r="J14">
+        <v>750</v>
+      </c>
+      <c r="K14">
+        <v>100</v>
+      </c>
+      <c r="L14">
+        <v>0.85</v>
+      </c>
+      <c r="M14">
+        <v>0.2</v>
+      </c>
+      <c r="N14">
+        <v>256</v>
+      </c>
+      <c r="O14">
+        <v>5</v>
+      </c>
+      <c r="P14">
+        <v>0.3</v>
+      </c>
+      <c r="Q14">
+        <v>0.99</v>
+      </c>
+      <c r="R14">
+        <v>1e-05</v>
+      </c>
+      <c r="S14" t="b">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="V14">
+        <v>8</v>
+      </c>
+      <c r="X14" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z14">
+        <v>1.5</v>
+      </c>
+      <c r="AA14">
+        <v>1</v>
+      </c>
+      <c r="AB14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28">
+      <c r="A15">
+        <v>48</v>
+      </c>
+      <c r="B15">
+        <v>1935.851388888889</v>
+      </c>
+      <c r="C15">
+        <v>17.21383332411448</v>
+      </c>
+      <c r="D15">
+        <v>418.9983333333334</v>
+      </c>
+      <c r="E15">
+        <v>200</v>
+      </c>
+      <c r="F15">
+        <v>2048</v>
+      </c>
+      <c r="G15">
+        <v>48</v>
+      </c>
+      <c r="H15">
+        <v>30</v>
+      </c>
+      <c r="I15">
+        <v>900</v>
+      </c>
+      <c r="J15">
+        <v>750</v>
+      </c>
+      <c r="K15">
+        <v>100</v>
+      </c>
+      <c r="L15">
+        <v>0.85</v>
+      </c>
+      <c r="M15">
+        <v>0.2</v>
+      </c>
+      <c r="N15">
+        <v>256</v>
+      </c>
+      <c r="O15">
+        <v>5</v>
+      </c>
+      <c r="P15">
+        <v>0.3</v>
+      </c>
+      <c r="Q15">
+        <v>0.99</v>
+      </c>
+      <c r="R15">
+        <v>1e-05</v>
+      </c>
+      <c r="S15" t="b">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15">
+        <v>8</v>
+      </c>
+      <c r="X15" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z15">
+        <v>1.5</v>
+      </c>
+      <c r="AA15">
+        <v>1</v>
+      </c>
+      <c r="AB15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28">
+      <c r="A16">
+        <v>48</v>
+      </c>
+      <c r="B16">
+        <v>1916.636111111111</v>
+      </c>
+      <c r="C16">
+        <v>30.3534051378568</v>
+      </c>
+      <c r="D16">
+        <v>385.5760416666665</v>
+      </c>
+      <c r="E16">
+        <v>400</v>
+      </c>
+      <c r="F16">
+        <v>2048</v>
+      </c>
+      <c r="G16">
+        <v>48</v>
+      </c>
+      <c r="H16">
+        <v>30</v>
+      </c>
+      <c r="I16">
+        <v>900</v>
+      </c>
+      <c r="J16">
+        <v>750</v>
+      </c>
+      <c r="K16">
+        <v>100</v>
+      </c>
+      <c r="L16">
+        <v>0.85</v>
+      </c>
+      <c r="M16">
+        <v>0.2</v>
+      </c>
+      <c r="N16">
+        <v>256</v>
+      </c>
+      <c r="O16">
+        <v>5</v>
+      </c>
+      <c r="P16">
+        <v>0.3</v>
+      </c>
+      <c r="Q16">
+        <v>0.99</v>
+      </c>
+      <c r="R16">
+        <v>1e-05</v>
+      </c>
+      <c r="S16" t="b">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="U16">
+        <v>1</v>
+      </c>
+      <c r="V16">
+        <v>8</v>
+      </c>
+      <c r="X16" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z16">
+        <v>1.5</v>
+      </c>
+      <c r="AA16">
+        <v>1</v>
+      </c>
+      <c r="AB16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28">
+      <c r="A17">
+        <v>408</v>
+      </c>
+      <c r="B17">
+        <v>1945.520833333333</v>
+      </c>
+      <c r="C17">
+        <v>30.45326904853185</v>
+      </c>
+      <c r="D17">
+        <v>407.1260416666668</v>
+      </c>
+      <c r="E17">
+        <v>400</v>
+      </c>
+      <c r="F17">
+        <v>2048</v>
+      </c>
+      <c r="G17">
+        <v>48</v>
+      </c>
+      <c r="H17">
+        <v>30</v>
+      </c>
+      <c r="I17">
+        <v>900</v>
+      </c>
+      <c r="J17">
+        <v>750</v>
+      </c>
+      <c r="K17">
+        <v>100</v>
+      </c>
+      <c r="L17">
+        <v>0.85</v>
+      </c>
+      <c r="M17">
+        <v>0.2</v>
+      </c>
+      <c r="N17">
+        <v>256</v>
+      </c>
+      <c r="O17">
+        <v>5</v>
+      </c>
+      <c r="P17">
+        <v>0.3</v>
+      </c>
+      <c r="Q17">
+        <v>0.99</v>
+      </c>
+      <c r="R17">
+        <v>1e-05</v>
+      </c>
+      <c r="S17" t="b">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="V17">
+        <v>8</v>
+      </c>
+      <c r="X17" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z17">
+        <v>1.5</v>
+      </c>
+      <c r="AA17">
+        <v>1</v>
+      </c>
+      <c r="AB17">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added independent distributed PPO multi-agent algorithm
</commit_message>
<xml_diff>
--- a/run-data.xlsx
+++ b/run-data.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+  <si>
+    <t>rollout</t>
+  </si>
+  <si>
+    <t>waitingTime</t>
+  </si>
   <si>
     <t>time</t>
   </si>
@@ -22,9 +28,6 @@
     <t>rew</t>
   </si>
   <si>
-    <t>waitingTime</t>
-  </si>
-  <si>
     <t>E_num_train_rollouts</t>
   </si>
   <si>
@@ -46,55 +49,64 @@
     <t>E_test_num_eps</t>
   </si>
   <si>
-    <t>A_gae_tau</t>
-  </si>
-  <si>
-    <t>A_entropy_weight</t>
-  </si>
-  <si>
-    <t>A_minibatch_size</t>
-  </si>
-  <si>
-    <t>A_optimization_epochs</t>
-  </si>
-  <si>
-    <t>A_ppo_ratio_clip</t>
-  </si>
-  <si>
-    <t>A_discount</t>
-  </si>
-  <si>
-    <t>A_learning_rate</t>
-  </si>
-  <si>
-    <t>A_clip_grads</t>
-  </si>
-  <si>
-    <t>A_gradient_clip</t>
-  </si>
-  <si>
-    <t>A_value_loss_coef</t>
-  </si>
-  <si>
-    <t>O_num_agents</t>
-  </si>
-  <si>
-    <t>O_rule_set</t>
-  </si>
-  <si>
-    <t>O_rule_set_params</t>
+    <t>P_gae_tau</t>
+  </si>
+  <si>
+    <t>P_entropy_weight</t>
+  </si>
+  <si>
+    <t>P_minibatch_size</t>
+  </si>
+  <si>
+    <t>P_optimization_epochs</t>
+  </si>
+  <si>
+    <t>P_ppo_ratio_clip</t>
+  </si>
+  <si>
+    <t>P_discount</t>
+  </si>
+  <si>
+    <t>P_learning_rate</t>
+  </si>
+  <si>
+    <t>P_clip_grads</t>
+  </si>
+  <si>
+    <t>P_gradient_clip</t>
+  </si>
+  <si>
+    <t>P_value_loss_coef</t>
+  </si>
+  <si>
+    <t>R_rule_set</t>
+  </si>
+  <si>
+    <t>R_rule_set_params</t>
+  </si>
+  <si>
+    <t>O_num_workers</t>
   </si>
   <si>
     <t>O_environment</t>
   </si>
   <si>
-    <t>O_NS_mult</t>
-  </si>
-  <si>
-    <t>O_EW_mult</t>
-  </si>
-  <si>
-    <t>O_phase_end_offset</t>
+    <t>O_agent_type</t>
+  </si>
+  <si>
+    <t>O_single_agent</t>
+  </si>
+  <si>
+    <t>cycle</t>
+  </si>
+  <si>
+    <t>{'cycle_length': 20, 'NS_mult': 1.5, 'EW_mult': 1.0, 'phase_end_offset': 100}</t>
+  </si>
+  <si>
+    <t>4_intersections_rush_hour</t>
+  </si>
+  <si>
+    <t>ppo</t>
   </si>
 </sst>
 </file>
@@ -452,7 +464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -541,6 +553,89 @@
         <v>26</v>
       </c>
     </row>
+    <row r="2" spans="1:27">
+      <c r="A2">
+        <v>250</v>
+      </c>
+      <c r="B2">
+        <v>1769.131666666667</v>
+      </c>
+      <c r="C2">
+        <v>31.3077213605245</v>
+      </c>
+      <c r="D2">
+        <v>426.59525</v>
+      </c>
+      <c r="E2">
+        <v>400</v>
+      </c>
+      <c r="F2">
+        <v>2048</v>
+      </c>
+      <c r="G2">
+        <v>50</v>
+      </c>
+      <c r="H2">
+        <v>25</v>
+      </c>
+      <c r="I2">
+        <v>900</v>
+      </c>
+      <c r="J2">
+        <v>750</v>
+      </c>
+      <c r="K2">
+        <v>50</v>
+      </c>
+      <c r="L2">
+        <v>0.85</v>
+      </c>
+      <c r="M2">
+        <v>0.1</v>
+      </c>
+      <c r="N2">
+        <v>256</v>
+      </c>
+      <c r="O2">
+        <v>5</v>
+      </c>
+      <c r="P2">
+        <v>0.3</v>
+      </c>
+      <c r="Q2">
+        <v>0.99</v>
+      </c>
+      <c r="R2">
+        <v>0.0001</v>
+      </c>
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
+        <v>27</v>
+      </c>
+      <c r="W2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X2">
+        <v>8</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA2" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added reward interpolation for mix of local/global reward
</commit_message>
<xml_diff>
--- a/run-data.xlsx
+++ b/run-data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>rollout</t>
   </si>
@@ -97,16 +97,7 @@
     <t>O_single_agent</t>
   </si>
   <si>
-    <t>cycle</t>
-  </si>
-  <si>
-    <t>{'cycle_length': 20, 'NS_mult': 1.5, 'EW_mult': 1.0, 'phase_end_offset': 100}</t>
-  </si>
-  <si>
-    <t>4_intersections_rush_hour</t>
-  </si>
-  <si>
-    <t>ppo</t>
+    <t>O_reward_discount</t>
   </si>
 </sst>
 </file>
@@ -464,13 +455,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:AB1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -552,88 +543,8 @@
       <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:27">
-      <c r="A2">
-        <v>250</v>
-      </c>
-      <c r="B2">
-        <v>1769.131666666667</v>
-      </c>
-      <c r="C2">
-        <v>31.3077213605245</v>
-      </c>
-      <c r="D2">
-        <v>426.59525</v>
-      </c>
-      <c r="E2">
-        <v>400</v>
-      </c>
-      <c r="F2">
-        <v>2048</v>
-      </c>
-      <c r="G2">
-        <v>50</v>
-      </c>
-      <c r="H2">
-        <v>25</v>
-      </c>
-      <c r="I2">
-        <v>900</v>
-      </c>
-      <c r="J2">
-        <v>750</v>
-      </c>
-      <c r="K2">
-        <v>50</v>
-      </c>
-      <c r="L2">
-        <v>0.85</v>
-      </c>
-      <c r="M2">
-        <v>0.1</v>
-      </c>
-      <c r="N2">
-        <v>256</v>
-      </c>
-      <c r="O2">
-        <v>5</v>
-      </c>
-      <c r="P2">
-        <v>0.3</v>
-      </c>
-      <c r="Q2">
-        <v>0.99</v>
-      </c>
-      <c r="R2">
-        <v>0.0001</v>
-      </c>
-      <c r="S2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <v>1</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="W2" t="s">
-        <v>28</v>
-      </c>
-      <c r="X2">
-        <v>8</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA2" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added scalable phases function
</commit_message>
<xml_diff>
--- a/run-data.xlsx
+++ b/run-data.xlsx
@@ -14,39 +14,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t>rollout</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>rew</t>
   </si>
   <si>
     <t>waitingTime</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>rew</t>
-  </si>
-  <si>
-    <t>E_num_train_rollouts</t>
-  </si>
-  <si>
-    <t>E_rollout_length</t>
-  </si>
-  <si>
-    <t>E_eval_freq</t>
-  </si>
-  <si>
-    <t>E_eval_num_eps</t>
-  </si>
-  <si>
-    <t>E_max_ep_steps</t>
-  </si>
-  <si>
-    <t>E_generation_ep_steps</t>
-  </si>
-  <si>
-    <t>E_test_num_eps</t>
+    <t>Ep_num_train_rollouts</t>
+  </si>
+  <si>
+    <t>Ep_rollout_length</t>
+  </si>
+  <si>
+    <t>Ep_eval_freq</t>
+  </si>
+  <si>
+    <t>Ep_eval_num_eps</t>
+  </si>
+  <si>
+    <t>Ep_max_ep_steps</t>
+  </si>
+  <si>
+    <t>Ep_generation_ep_steps</t>
+  </si>
+  <si>
+    <t>Ep_test_num_eps</t>
+  </si>
+  <si>
+    <t>A_agent_type</t>
+  </si>
+  <si>
+    <t>A_single_agent</t>
   </si>
   <si>
     <t>P_gae_tau</t>
@@ -85,19 +88,22 @@
     <t>R_rule_set_params</t>
   </si>
   <si>
-    <t>O_num_workers</t>
-  </si>
-  <si>
-    <t>O_environment</t>
-  </si>
-  <si>
-    <t>O_agent_type</t>
-  </si>
-  <si>
-    <t>O_single_agent</t>
-  </si>
-  <si>
-    <t>O_reward_interpolation</t>
+    <t>En_shape</t>
+  </si>
+  <si>
+    <t>En_rush_hour</t>
+  </si>
+  <si>
+    <t>En_uniform_generation_probability</t>
+  </si>
+  <si>
+    <t>M_reward_interpolation</t>
+  </si>
+  <si>
+    <t>M_state_interpolation</t>
+  </si>
+  <si>
+    <t>P_num_workers</t>
   </si>
 </sst>
 </file>
@@ -455,13 +461,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB1"/>
+  <dimension ref="A1:AD1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,6 +551,12 @@
       </c>
       <c r="AB1" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>